<commit_message>
created a patterns folder for level patterns we want to save, deleting level0/1 from the repo now
</commit_message>
<xml_diff>
--- a/core/assets/levels/level0.xlsx
+++ b/core/assets/levels/level0.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stsinwell/cs/MangoSnoopers/core/assets/levels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA172A7-A0BC-4F44-A235-B1CDF65E3C4C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6870" yWindow="660" windowWidth="29460" windowHeight="22305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6880" yWindow="660" windowWidth="29460" windowHeight="22300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
   <si>
     <t>Events</t>
   </si>
@@ -387,8 +386,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -802,27 +801,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="29" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.875" style="2"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -848,7 +847,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -861,12 +860,11 @@
       <c r="D2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="16"/>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D3" s="6"/>
       <c r="E3"/>
       <c r="F3"/>
@@ -875,7 +873,7 @@
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -897,7 +895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -917,14 +915,14 @@
       </c>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D6" s="6"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>16</v>
       </c>
@@ -936,7 +934,7 @@
       <c r="G7"/>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -944,14 +942,13 @@
         <v>10</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8"/>
       <c r="F8" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
@@ -968,7 +965,7 @@
       </c>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -983,7 +980,7 @@
       </c>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -996,7 +993,7 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D12" s="6"/>
       <c r="E12"/>
       <c r="F12"/>
@@ -1005,7 +1002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D13" s="6"/>
       <c r="E13"/>
       <c r="F13"/>
@@ -1014,7 +1011,7 @@
       </c>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -1028,7 +1025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -1040,7 +1037,7 @@
       </c>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -1050,7 +1047,7 @@
       <c r="G16" s="12"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
@@ -1062,7 +1059,7 @@
       <c r="G17"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
@@ -1074,7 +1071,7 @@
       <c r="G18"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8" ht="21">
+    <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>7</v>
       </c>
@@ -1090,7 +1087,7 @@
       </c>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -1102,7 +1099,7 @@
       </c>
       <c r="H20"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>3</v>
       </c>
@@ -1116,7 +1113,7 @@
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>40</v>
       </c>
@@ -1130,7 +1127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>24</v>
       </c>
@@ -1144,7 +1141,7 @@
       </c>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
@@ -1158,7 +1155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
@@ -1172,7 +1169,7 @@
       </c>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
@@ -1183,220 +1180,358 @@
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27"/>
       <c r="F27"/>
       <c r="G27"/>
-      <c r="H27"/>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="H27" s="12"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="F29" s="12"/>
+      <c r="E29" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29"/>
       <c r="G29" s="12"/>
-    </row>
-    <row r="30" spans="1:8" s="6" customFormat="1">
+      <c r="H29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="H31" s="12"/>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="E32"/>
+      <c r="F32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32"/>
+      <c r="H32"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
+      <c r="F33" t="s">
+        <v>4</v>
+      </c>
       <c r="G33" s="12"/>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>50</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="E34" t="s">
+        <v>58</v>
+      </c>
+      <c r="F34"/>
+      <c r="G34" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="F36" s="12"/>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37" s="12"/>
+      <c r="H37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38" t="s">
+        <v>4</v>
+      </c>
+      <c r="H38"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="E39" t="s">
+        <v>59</v>
+      </c>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40" t="s">
+        <v>4</v>
+      </c>
+      <c r="H40"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41" s="12"/>
+      <c r="H41"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="E42"/>
+      <c r="F42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42"/>
+      <c r="H42"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="E43"/>
+      <c r="F43" t="s">
+        <v>4</v>
+      </c>
+      <c r="G43"/>
+      <c r="H43"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
-      <c r="G44" s="12"/>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="E44" t="s">
+        <v>57</v>
+      </c>
+      <c r="F44"/>
+      <c r="G44" t="s">
+        <v>4</v>
+      </c>
+      <c r="H44"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45" t="s">
+        <v>4</v>
+      </c>
+      <c r="H45"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="E46" t="s">
+        <v>60</v>
+      </c>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48" t="s">
+        <v>4</v>
+      </c>
+      <c r="H48"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50" t="s">
+        <v>4</v>
+      </c>
+      <c r="H50"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>22</v>
       </c>
@@ -1404,7 +1539,7 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>23</v>
       </c>
@@ -1412,13 +1547,13 @@
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>

</xml_diff>